<commit_message>
added fips to beginning of tract numbers
</commit_message>
<xml_diff>
--- a/acs/elections_with_tracts.xlsx
+++ b/acs/elections_with_tracts.xlsx
@@ -4318,7 +4318,7 @@
       <c r="J94" t="inlineStr"/>
       <c r="K94" t="inlineStr">
         <is>
-          <t>[4200, 4100, 600, 900, 200, 300, 1000]</t>
+          <t>['50_007_004200', '50_007_004100', '50_007_000600', '50_007_000900', '50_007_000200', '50_007_000300', '50_007_001000']</t>
         </is>
       </c>
       <c r="L94" t="inlineStr">
@@ -4374,7 +4374,7 @@
       <c r="J95" t="inlineStr"/>
       <c r="K95" t="inlineStr">
         <is>
-          <t>[4200, 3600, 3900, 2502, 4100, 600, 900, 300, 1000]</t>
+          <t>['50_007_004200', '50_007_003600', '50_007_003900', '50_007_002502', '50_007_004100', '50_007_000600', '50_007_000900', '50_007_000300', '50_007_001000']</t>
         </is>
       </c>
       <c r="L95" t="inlineStr">
@@ -4430,7 +4430,7 @@
       <c r="J96" t="inlineStr"/>
       <c r="K96" t="inlineStr">
         <is>
-          <t>[3600, 3900, 3304, 800, 900, 1100, 1000]</t>
+          <t>['50_007_003600', '50_007_003900', '50_007_003304', '50_007_000800', '50_007_000900', '50_007_001100', '50_007_001000']</t>
         </is>
       </c>
       <c r="L96" t="inlineStr">
@@ -4522,7 +4522,7 @@
       <c r="J98" t="inlineStr"/>
       <c r="K98" t="inlineStr">
         <is>
-          <t>[1102, 700, 800, 900, 1000, 1204, 1104, 1103, 201, 1203, 1205]</t>
+          <t>['35_013_001102', '35_013_000700', '35_013_000800', '35_013_000900', '35_013_001000', '35_013_001204', '35_013_001104', '35_013_001103', '35_013_000201', '35_013_001203', '35_013_001205']</t>
         </is>
       </c>
       <c r="L98" t="inlineStr">
@@ -4576,7 +4576,7 @@
       <c r="J99" t="inlineStr"/>
       <c r="K99" t="inlineStr">
         <is>
-          <t>[1500, 1102, 300, 500, 600, 202, 201, 103]</t>
+          <t>['35_013_001500', '35_013_001102', '35_013_000300', '35_013_000500', '35_013_000600', '35_013_000202', '35_013_000201', '35_013_000103']</t>
         </is>
       </c>
       <c r="L99" t="inlineStr">
@@ -14152,7 +14152,7 @@
       <c r="J279" t="inlineStr"/>
       <c r="K279" t="inlineStr">
         <is>
-          <t>[952900, 950900, 952100, 952300, 951200, 951300, 951400, 951100, 950100, 952700, 950700, 951700, 950600, 950400, 950200, 952600, 952400, 952500, 951600, 950300, 951000, 951800, 951900, 952000, 956300, 956400, 955300, 955400, 955900, 955500, 956500, 955100, 955800, 956100, 955700, 956200, 955600, 990000, 965100, 965900, 966300, 966500, 965300, 966400, 966100, 965200, 966600, 21500, 200, 300, 400, 500, 600, 700, 900, 20500, 8001, 4100, 4200, 4300, 27000, 11000, 25500, 26500, 9000, 14000, 15000, 12500, 31000, 28000, 13500, 15500, 22500, 2000, 10000, 12000, 28500, 24500, 18000, 29000, 30000, 13000, 7100, 7200, 6200, 6100, 6300, 3000, 5000, 940000, 31300, 31100, 31200, 965700, 965400, 966200, 965800, 966000, 965504, 965503, 990000, 966700, 46001, 46002, 41000, 44000, 47000, 45000, 43000, 42000, 22500, 970601, 970101, 970602, 970102, 971200, 971400, 971300, 971000, 971100, 965301, 965302, 966700, 966600, 966000, 966900, 967000, 966500, 965900, 966800, 965800, 966300, 966100, 965700, 966200, 965600, 966400, 966100, 966900, 966200, 966300, 966500, 965600, 966400, 965800, 965900, 966600, 965500, 966800, 966000, 965700, 965100, 966700, 965400, 18000, 17000, 25000, 15500, 13000, 14000, 12000, 11000, 15000, 14500, 10900, 21000, 20000, 10600, 22000, 16000, 23002, 10801, 20500, 970301, 970100, 970200, 960302, 960301, 960600, 960700, 960900, 960400, 960800, 960500, 970300, 42000, 43000, 20500, 40000, 44000, 41500, 20800, 20700, 41000, 20300, 20400, 46000, 20600, 45000, 30100, 20200, 20900, 10800, 10100, 10400, 10200, 10700, 10500, 30200, 10600, 10300, 46500, 20100, 11500, 14000, 13000, 16500, 16000, 15000, 10802, 24200]</t>
+          <t>['23_003_952900', '23_003_950900', '23_003_952100', '23_003_952300', '23_003_951200', '23_003_951300', '23_003_951400', '23_003_951100', '23_003_950100', '23_003_952700', '23_003_950700', '23_003_951700', '23_003_950600', '23_003_950400', '23_003_950200', '23_003_952600', '23_003_952400', '23_003_952500', '23_003_951600', '23_003_950300', '23_003_951000', '23_003_951800', '23_003_951900', '23_003_952000', '23_029_956300', '23_029_956400', '23_029_955300', '23_029_955400', '23_029_955900', '23_029_955500', '23_029_956500', '23_029_955100', '23_029_955800', '23_029_956100', '23_029_955700', '23_029_956200', '23_029_955600', '23_029_990000', '23_009_965100', '23_009_965900', '23_009_966300', '23_009_966500', '23_009_965300', '23_009_966400', '23_009_966100', '23_009_965200', '23_009_966600', '23_019_021500', '23_019_000200', '23_019_000300', '23_019_000400', '23_019_000500', '23_019_000600', '23_019_000700', '23_019_000900', '23_019_020500', '23_019_008001', '23_019_004100', '23_019_004200', '23_019_004300', '23_019_027000', '23_019_011000', '23_019_025500', '23_019_026500', '23_019_009000', '23_019_014000', '23_019_015000', '23_019_012500', '23_019_031000', '23_019_028000', '23_019_013500', '23_019_015500', '23_019_022500', '23_019_002000', '23_019_010000', '23_019_012000', '23_019_028500', '23_019_024500', '23_019_018000', '23_019_029000', '23_019_030000', '23_019_013000', '23_019_007100', '23_019_007200', '23_019_006200', '23_019_006100', '23_019_006300', '23_019_003000', '23_019_005000', '23_019_940000', '23_019_031300', '23_019_031100', '23_019_031200', '23_009_965700', '23_009_965400', '23_009_966200', '23_009_965800', '23_009_966000', '23_009_965504', '23_009_965503', '23_009_990000', '23_009_966700', '23_027_046001', '23_027_046002', '23_027_041000', '23_027_044000', '23_027_047000', '23_027_045000', '23_027_043000', '23_027_042000', '23_031_022500', '23_007_970601', '23_007_970101', '23_007_970602', '23_007_970102', '23_007_971200', '23_007_971400', '23_007_971300', '23_007_971000', '23_007_971100', '23_025_965301', '23_025_965302', '23_025_966700', '23_025_966600', '23_025_966000', '23_025_966900', '23_025_967000', '23_025_966500', '23_025_965900', '23_025_966800', '23_025_965800', '23_025_966300', '23_025_966100', '23_025_965700', '23_025_966200', '23_025_965600', '23_025_966400', '23_017_966100', '23_017_966900', '23_017_966200', '23_017_966300', '23_017_966500', '23_017_965600', '23_017_966400', '23_017_965800', '23_017_965900', '23_017_966600', '23_017_965500', '23_017_966800', '23_017_966000', '23_017_965700', '23_017_965100', '23_017_966700', '23_017_965400', '23_011_018000', '23_011_017000', '23_011_025000', '23_011_015500', '23_011_013000', '23_011_014000', '23_011_012000', '23_011_011000', '23_011_015000', '23_011_014500', '23_011_010900', '23_011_021000', '23_011_020000', '23_011_010600', '23_011_022000', '23_011_016000', '23_011_023002', '23_011_010801', '23_011_020500', '23_023_970301', '23_023_970100', '23_023_970200', '23_021_960302', '23_021_960301', '23_021_960600', '23_021_960700', '23_021_960900', '23_021_960400', '23_021_960800', '23_021_960500', '23_013_970300', '23_001_042000', '23_001_043000', '23_001_020500', '23_001_040000', '23_001_044000', '23_001_041500', '23_001_020800', '23_001_020700', '23_001_041000', '23_001_020300', '23_001_020400', '23_001_046000', '23_001_020600', '23_001_045000', '23_001_030100', '23_001_020200', '23_001_020900', '23_001_010800', '23_001_010100', '23_001_010400', '23_001_010200', '23_001_010700', '23_001_010500', '23_001_030200', '23_001_010600', '23_001_010300', '23_001_046500', '23_001_020100', '23_005_011500', '23_005_014000', '23_005_013000', '23_005_016500', '23_005_016000', '23_005_015000', '23_011_010802', '23_011_024200']</t>
         </is>
       </c>
       <c r="L279" t="inlineStr">
@@ -14202,7 +14202,7 @@
       <c r="J280" t="inlineStr"/>
       <c r="K280" t="inlineStr">
         <is>
-          <t>[3000, 4100, 4300, 5000, 6100, 6300, 11000, 12000, 43000, 13000, 18000, 9000, 20500, 2000, 8001, 13500, 22500, 29000, 960800, 960700, 960600, 960400, 960500, 960900, 966800, 966600, 965800, 966900, 965100, 965600, 966100, 966300, 965500, 966700, 965400, 965700, 966402, 966002, 966401, 966001, 970200, 966500, 11000, 24500, 31000, 400, 500, 600, 20500, 22000, 965300, 965100, 965800, 966300, 966400, 966600, 965700, 965400, 966200, 965900, 965900, 966200, 966100, 40000, 46000, 46500, 990000, 10100, 10300, 10400, 970302, 970301, 10500, 20100, 20200, 20500, 20600, 20900, 45000, 41000, 43000, 41500, 30200, 10600, 42000, 30100, 20700, 10700, 10200, 10800, 970101, 970601, 970301, 970100, 22500, 14500, 18000, 28500, 28000, 300, 10900, 27000, 15500, 6200, 700, 15000, 14000, 12500, 7100, 4200, 26500, 900, 7200, 30000, 21500, 25500, 10000, 200, 965504, 965503, 966700, 966000, 966500, 956200, 956400, 955400, 955900, 45000, 41000, 42000, 44000, 47000, 966100, 970102, 965700, 966702, 966601, 966602, 966701, 966802, 966801, 966900, 971202, 971201, 20303, 20301, 20802, 20801, 20402, 20302, 20401, 15000, 952700, 952600, 952900, 952300, 950400, 951400, 950700, 950600, 950100, 951800, 952000, 951900, 951200, 950300, 970602, 950900, 951000, 951100, 965900, 965600, 966200, 966000, 967000, 951600, 951700, 13000, 21000, 16000, 12000, 17000, 10801, 20000, 15500, 952400, 952500, 950200, 951300, 952100, 16001, 14001, 13001, 966400, 965200, 965800, 966500, 955100, 955500, 955800, 956100, 956500, 955700, 955600, 956300, 955300, 44000, 940000, 31300, 31100, 31200, 966300, 23002, 14002, 14001, 10601, 25001, 25002, 10804, 10803, 24202, 10602, 971000, 971300, 971100, 971400, 46002, 46001, 960301, 960302, 11500, 15000, 16500, 965302, 965301, 990000]</t>
+          <t>['23_019_003000', '23_019_004100', '23_019_004300', '23_019_005000', '23_019_006100', '23_019_006300', '23_019_011000', '23_019_012000', '23_027_043000', '23_019_013000', '23_019_018000', '23_019_009000', '23_019_020500', '23_019_002000', '23_019_008001', '23_019_013500', '23_019_022500', '23_019_029000', '23_021_960800', '23_021_960700', '23_021_960600', '23_021_960400', '23_021_960500', '23_021_960900', '23_017_966800', '23_017_966600', '23_017_965800', '23_017_966900', '23_017_965100', '23_017_965600', '23_017_966100', '23_017_966300', '23_017_965500', '23_017_966700', '23_017_965400', '23_017_965700', '23_017_966402', '23_017_966002', '23_017_966401', '23_017_966001', '23_023_970200', '23_017_966500', '23_011_011000', '23_019_024500', '23_019_031000', '23_019_000400', '23_019_000500', '23_019_000600', '23_011_020500', '23_011_022000', '23_009_965300', '23_009_965100', '23_009_965800', '23_009_966300', '23_009_966400', '23_009_966600', '23_009_965700', '23_009_965400', '23_009_966200', '23_009_965900', '23_017_965900', '23_017_966200', '23_009_966100', '23_001_040000', '23_001_046000', '23_001_046500', '23_029_990000', '23_001_010100', '23_001_010300', '23_001_010400', '23_013_970302', '23_013_970301', '23_001_010500', '23_001_020100', '23_001_020200', '23_001_020500', '23_001_020600', '23_001_020900', '23_001_045000', '23_001_041000', '23_001_043000', '23_001_041500', '23_001_030200', '23_001_010600', '23_001_042000', '23_001_030100', '23_001_020700', '23_001_010700', '23_001_010200', '23_001_010800', '23_007_970101', '23_007_970601', '23_023_970301', '23_023_970100', '23_031_022500', '23_011_014500', '23_011_018000', '23_019_028500', '23_019_028000', '23_019_000300', '23_011_010900', '23_019_027000', '23_019_015500', '23_019_006200', '23_019_000700', '23_019_015000', '23_019_014000', '23_019_012500', '23_019_007100', '23_019_004200', '23_019_026500', '23_019_000900', '23_019_007200', '23_019_030000', '23_019_021500', '23_019_025500', '23_019_010000', '23_019_000200', '23_009_965504', '23_009_965503', '23_009_966700', '23_009_966000', '23_009_966500', '23_029_956200', '23_029_956400', '23_029_955400', '23_029_955900', '23_027_045000', '23_027_041000', '23_027_042000', '23_027_044000', '23_027_047000', '23_025_966100', '23_007_970102', '23_025_965700', '23_025_966702', '23_025_966601', '23_025_966602', '23_025_966701', '23_025_966802', '23_025_966801', '23_025_966900', '23_007_971202', '23_007_971201', '23_001_020303', '23_001_020301', '23_001_020802', '23_001_020801', '23_001_020402', '23_001_020302', '23_001_020401', '23_011_015000', '23_003_952700', '23_003_952600', '23_003_952900', '23_003_952300', '23_003_950400', '23_003_951400', '23_003_950700', '23_003_950600', '23_003_950100', '23_003_951800', '23_003_952000', '23_003_951900', '23_003_951200', '23_003_950300', '23_007_970602', '23_003_950900', '23_003_951000', '23_003_951100', '23_025_965900', '23_025_965600', '23_025_966200', '23_025_966000', '23_025_967000', '23_003_951600', '23_003_951700', '23_011_013000', '23_011_021000', '23_011_016000', '23_011_012000', '23_011_017000', '23_011_010801', '23_011_020000', '23_011_015500', '23_003_952400', '23_003_952500', '23_003_950200', '23_003_951300', '23_003_952100', '23_005_016001', '23_005_014001', '23_005_013001', '23_025_966400', '23_009_965200', '23_025_965800', '23_025_966500', '23_029_955100', '23_029_955500', '23_029_955800', '23_029_956100', '23_029_956500', '23_029_955700', '23_029_955600', '23_029_956300', '23_029_955300', '23_001_044000', '23_019_940000', '23_019_031300', '23_019_031100', '23_019_031200', '23_025_966300', '23_011_023002', '23_011_014002', '23_011_014001', '23_011_010601', '23_011_025001', '23_011_025002', '23_011_010804', '23_011_010803', '23_011_024202', '23_011_010602', '23_007_971000', '23_007_971300', '23_007_971100', '23_007_971400', '23_027_046002', '23_027_046001', '23_021_960301', '23_021_960302', '23_005_011500', '23_005_015000', '23_005_016500', '23_025_965302', '23_025_965301', '23_009_990000']</t>
         </is>
       </c>
       <c r="L280" t="inlineStr">
@@ -14252,7 +14252,7 @@
       <c r="J281" t="inlineStr"/>
       <c r="K281" t="inlineStr">
         <is>
-          <t>[952900, 950900, 952100, 952300, 951200, 951300, 951400, 951100, 950100, 952700, 950700, 951700, 950600, 950400, 950200, 952600, 952400, 952500, 951600, 950300, 951000, 951800, 951900, 952000, 956300, 956400, 955300, 955400, 955900, 955500, 956500, 955100, 955800, 956100, 955700, 956200, 955600, 990000, 965100, 965900, 966300, 966500, 965300, 966400, 966100, 965200, 966600, 21500, 200, 300, 400, 500, 600, 700, 900, 20500, 8001, 4100, 4200, 4300, 27000, 11000, 25500, 26500, 9000, 14000, 15000, 12500, 31000, 28000, 13500, 15500, 22500, 2000, 10000, 12000, 28500, 24500, 18000, 29000, 30000, 13000, 7100, 7200, 6200, 6100, 6300, 3000, 5000, 940000, 31300, 31100, 31200, 965700, 965400, 966200, 965800, 966000, 965504, 965503, 990000, 966700, 46001, 46002, 41000, 44000, 47000, 45000, 43000, 42000, 22500, 970601, 970101, 970602, 970102, 971200, 971400, 971300, 971000, 971100, 965301, 965302, 966700, 966600, 966000, 966900, 967000, 966500, 965900, 966800, 965800, 966300, 966100, 965700, 966200, 965600, 966400, 966100, 966900, 966200, 966300, 966500, 965600, 966400, 965800, 965900, 966600, 965500, 966800, 966000, 965700, 965100, 966700, 965400, 18000, 17000, 25000, 15500, 13000, 14000, 12000, 11000, 15000, 14500, 10900, 21000, 20000, 10600, 22000, 16000, 23002, 10801, 20500, 970301, 970100, 970200, 960302, 960301, 960600, 960700, 960900, 960400, 960800, 960500, 970300, 42000, 43000, 20500, 40000, 44000, 41500, 20800, 20700, 41000, 20300, 20400, 46000, 20600, 45000, 30100, 20200, 20900, 10800, 10100, 10400, 10200, 10700, 10500, 30200, 10600, 10300, 46500, 20100, 11500, 14000, 13000, 16500, 16000, 15000, 10802, 24200]</t>
+          <t>['23_003_952900', '23_003_950900', '23_003_952100', '23_003_952300', '23_003_951200', '23_003_951300', '23_003_951400', '23_003_951100', '23_003_950100', '23_003_952700', '23_003_950700', '23_003_951700', '23_003_950600', '23_003_950400', '23_003_950200', '23_003_952600', '23_003_952400', '23_003_952500', '23_003_951600', '23_003_950300', '23_003_951000', '23_003_951800', '23_003_951900', '23_003_952000', '23_029_956300', '23_029_956400', '23_029_955300', '23_029_955400', '23_029_955900', '23_029_955500', '23_029_956500', '23_029_955100', '23_029_955800', '23_029_956100', '23_029_955700', '23_029_956200', '23_029_955600', '23_029_990000', '23_009_965100', '23_009_965900', '23_009_966300', '23_009_966500', '23_009_965300', '23_009_966400', '23_009_966100', '23_009_965200', '23_009_966600', '23_019_021500', '23_019_000200', '23_019_000300', '23_019_000400', '23_019_000500', '23_019_000600', '23_019_000700', '23_019_000900', '23_019_020500', '23_019_008001', '23_019_004100', '23_019_004200', '23_019_004300', '23_019_027000', '23_019_011000', '23_019_025500', '23_019_026500', '23_019_009000', '23_019_014000', '23_019_015000', '23_019_012500', '23_019_031000', '23_019_028000', '23_019_013500', '23_019_015500', '23_019_022500', '23_019_002000', '23_019_010000', '23_019_012000', '23_019_028500', '23_019_024500', '23_019_018000', '23_019_029000', '23_019_030000', '23_019_013000', '23_019_007100', '23_019_007200', '23_019_006200', '23_019_006100', '23_019_006300', '23_019_003000', '23_019_005000', '23_019_940000', '23_019_031300', '23_019_031100', '23_019_031200', '23_009_965700', '23_009_965400', '23_009_966200', '23_009_965800', '23_009_966000', '23_009_965504', '23_009_965503', '23_009_990000', '23_009_966700', '23_027_046001', '23_027_046002', '23_027_041000', '23_027_044000', '23_027_047000', '23_027_045000', '23_027_043000', '23_027_042000', '23_031_022500', '23_007_970601', '23_007_970101', '23_007_970602', '23_007_970102', '23_007_971200', '23_007_971400', '23_007_971300', '23_007_971000', '23_007_971100', '23_025_965301', '23_025_965302', '23_025_966700', '23_025_966600', '23_025_966000', '23_025_966900', '23_025_967000', '23_025_966500', '23_025_965900', '23_025_966800', '23_025_965800', '23_025_966300', '23_025_966100', '23_025_965700', '23_025_966200', '23_025_965600', '23_025_966400', '23_017_966100', '23_017_966900', '23_017_966200', '23_017_966300', '23_017_966500', '23_017_965600', '23_017_966400', '23_017_965800', '23_017_965900', '23_017_966600', '23_017_965500', '23_017_966800', '23_017_966000', '23_017_965700', '23_017_965100', '23_017_966700', '23_017_965400', '23_011_018000', '23_011_017000', '23_011_025000', '23_011_015500', '23_011_013000', '23_011_014000', '23_011_012000', '23_011_011000', '23_011_015000', '23_011_014500', '23_011_010900', '23_011_021000', '23_011_020000', '23_011_010600', '23_011_022000', '23_011_016000', '23_011_023002', '23_011_010801', '23_011_020500', '23_023_970301', '23_023_970100', '23_023_970200', '23_021_960302', '23_021_960301', '23_021_960600', '23_021_960700', '23_021_960900', '23_021_960400', '23_021_960800', '23_021_960500', '23_013_970300', '23_001_042000', '23_001_043000', '23_001_020500', '23_001_040000', '23_001_044000', '23_001_041500', '23_001_020800', '23_001_020700', '23_001_041000', '23_001_020300', '23_001_020400', '23_001_046000', '23_001_020600', '23_001_045000', '23_001_030100', '23_001_020200', '23_001_020900', '23_001_010800', '23_001_010100', '23_001_010400', '23_001_010200', '23_001_010700', '23_001_010500', '23_001_030200', '23_001_010600', '23_001_010300', '23_001_046500', '23_001_020100', '23_005_011500', '23_005_014000', '23_005_013000', '23_005_016500', '23_005_016000', '23_005_015000', '23_011_010802', '23_011_024200']</t>
         </is>
       </c>
       <c r="L281" t="inlineStr">
@@ -14302,7 +14302,7 @@
       <c r="J282" t="inlineStr"/>
       <c r="K282" t="inlineStr">
         <is>
-          <t>[11300, 3000, 4100, 4300, 5000, 6100, 6300, 11000, 12000, 43000, 13000, 18000, 9000, 20500, 2000, 8001, 13500, 22500, 29000, 960800, 960700, 960600, 960400, 960500, 960900, 966800, 966600, 965800, 966900, 965100, 965600, 966100, 966300, 965500, 966700, 965400, 965700, 966402, 966002, 966401, 966001, 970200, 966500, 11000, 23001, 24101, 970200, 24500, 31000, 400, 500, 600, 19000, 20500, 22000, 965300, 965100, 965800, 966300, 966400, 966600, 965700, 965400, 966200, 965900, 965900, 966200, 966100, 40000, 46000, 46500, 990000, 10100, 10300, 10400, 970302, 970301, 10500, 20100, 20200, 20500, 20600, 20900, 45000, 41000, 43000, 41500, 30200, 10600, 42000, 30100, 20700, 10700, 10200, 10800, 4501, 970101, 970601, 970301, 970100, 22500, 24102, 14500, 18000, 28500, 28000, 300, 10900, 27000, 15500, 6200, 700, 15000, 14000, 12500, 7100, 4200, 26500, 900, 7200, 30000, 21500, 25500, 10000, 200, 965504, 965503, 966700, 971100, 966000, 966500, 956200, 956400, 955400, 955900, 45000, 41000, 42000, 44000, 47000, 966100, 970102, 965700, 966702, 966601, 966602, 966701, 966802, 966801, 966900, 971202, 971201, 20303, 20301, 20802, 20801, 20402, 20302, 20401, 15000, 952700, 952600, 952900, 952300, 950400, 951400, 950700, 950600, 950100, 951800, 952000, 951900, 951200, 950300, 970602, 950900, 951000, 951100, 965900, 965600, 966200, 966000, 967000, 951600, 951700, 10300, 13000, 21000, 16000, 10200, 12000, 10500, 17000, 10801, 10100, 20000, 15500, 10700, 952400, 952500, 950200, 951300, 952100, 16002, 16001, 12001, 14001, 13001, 966400, 965200, 965800, 966500, 955100, 955500, 955800, 956100, 956500, 955700, 955600, 956300, 955300, 44000, 940000, 31300, 31100, 31200, 966300, 23002, 14002, 14001, 10601, 25001, 25002, 10804, 10803, 24202, 10602, 971000, 971300, 971100, 971400, 46002, 46001, 960301, 960302, 990000, 11500, 15000, 16500, 10400, 965302, 965301, 975100, 990000]</t>
+          <t>['23_005_011300', '23_019_003000', '23_019_004100', '23_019_004300', '23_019_005000', '23_019_006100', '23_019_006300', '23_019_011000', '23_019_012000', '23_027_043000', '23_019_013000', '23_019_018000', '23_019_009000', '23_019_020500', '23_019_002000', '23_019_008001', '23_019_013500', '23_019_022500', '23_019_029000', '23_021_960800', '23_021_960700', '23_021_960600', '23_021_960400', '23_021_960500', '23_021_960900', '23_017_966800', '23_017_966600', '23_017_965800', '23_017_966900', '23_017_965100', '23_017_965600', '23_017_966100', '23_017_966300', '23_017_965500', '23_017_966700', '23_017_965400', '23_017_965700', '23_017_966402', '23_017_966002', '23_017_966401', '23_017_966001', '23_023_970200', '23_017_966500', '23_011_011000', '23_011_023001', '23_011_024101', '23_013_970200', '23_019_024500', '23_019_031000', '23_019_000400', '23_019_000500', '23_019_000600', '23_011_019000', '23_011_020500', '23_011_022000', '23_009_965300', '23_009_965100', '23_009_965800', '23_009_966300', '23_009_966400', '23_009_966600', '23_009_965700', '23_009_965400', '23_009_966200', '23_009_965900', '23_017_965900', '23_017_966200', '23_009_966100', '23_001_040000', '23_001_046000', '23_001_046500', '23_029_990000', '23_001_010100', '23_001_010300', '23_001_010400', '23_013_970302', '23_013_970301', '23_001_010500', '23_001_020100', '23_001_020200', '23_001_020500', '23_001_020600', '23_001_020900', '23_001_045000', '23_001_041000', '23_001_043000', '23_001_041500', '23_001_030200', '23_001_010600', '23_001_042000', '23_001_030100', '23_001_020700', '23_001_010700', '23_001_010200', '23_001_010800', '23_005_004501', '23_007_970101', '23_007_970601', '23_023_970301', '23_023_970100', '23_031_022500', '23_011_024102', '23_011_014500', '23_011_018000', '23_019_028500', '23_019_028000', '23_019_000300', '23_011_010900', '23_019_027000', '23_019_015500', '23_019_006200', '23_019_000700', '23_019_015000', '23_019_014000', '23_019_012500', '23_019_007100', '23_019_004200', '23_019_026500', '23_019_000900', '23_019_007200', '23_019_030000', '23_019_021500', '23_019_025500', '23_019_010000', '23_019_000200', '23_009_965504', '23_009_965503', '23_009_966700', '23_013_971100', '23_009_966000', '23_009_966500', '23_029_956200', '23_029_956400', '23_029_955400', '23_029_955900', '23_027_045000', '23_027_041000', '23_027_042000', '23_027_044000', '23_027_047000', '23_025_966100', '23_007_970102', '23_025_965700', '23_025_966702', '23_025_966601', '23_025_966602', '23_025_966701', '23_025_966802', '23_025_966801', '23_025_966900', '23_007_971202', '23_007_971201', '23_001_020303', '23_001_020301', '23_001_020802', '23_001_020801', '23_001_020402', '23_001_020302', '23_001_020401', '23_011_015000', '23_003_952700', '23_003_952600', '23_003_952900', '23_003_952300', '23_003_950400', '23_003_951400', '23_003_950700', '23_003_950600', '23_003_950100', '23_003_951800', '23_003_952000', '23_003_951900', '23_003_951200', '23_003_950300', '23_007_970602', '23_003_950900', '23_003_951000', '23_003_951100', '23_025_965900', '23_025_965600', '23_025_966200', '23_025_966000', '23_025_967000', '23_003_951600', '23_003_951700', '23_011_010300', '23_011_013000', '23_011_021000', '23_011_016000', '23_011_010200', '23_011_012000', '23_011_010500', '23_011_017000', '23_011_010801', '23_011_010100', '23_011_020000', '23_011_015500', '23_011_010700', '23_003_952400', '23_003_952500', '23_003_950200', '23_003_951300', '23_003_952100', '23_005_016002', '23_005_016001', '23_005_012001', '23_005_014001', '23_005_013001', '23_025_966400', '23_009_965200', '23_025_965800', '23_025_966500', '23_029_955100', '23_029_955500', '23_029_955800', '23_029_956100', '23_029_956500', '23_029_955700', '23_029_955600', '23_029_956300', '23_029_955300', '23_001_044000', '23_019_940000', '23_019_031300', '23_019_031100', '23_019_031200', '23_025_966300', '23_011_023002', '23_011_014002', '23_011_014001', '23_011_010601', '23_011_025001', '23_011_025002', '23_011_010804', '23_011_010803', '23_011_024202', '23_011_010602', '23_007_971000', '23_007_971300', '23_007_971100', '23_007_971400', '23_027_046002', '23_027_046001', '23_021_960301', '23_021_960302', '23_013_990000', '23_005_011500', '23_005_015000', '23_005_016500', '23_011_010400', '23_025_965302', '23_025_965301', '23_015_975100', '23_009_990000']</t>
         </is>
       </c>
       <c r="L282" t="inlineStr">
@@ -15162,7 +15162,7 @@
       <c r="J299" t="inlineStr"/>
       <c r="K299" t="inlineStr">
         <is>
-          <t>[400, 102, 101, 300, 200, 200, 300, 300, 940100, 100]</t>
+          <t>['02_130_000400', '02_130_000102', '02_130_000101', '02_275_000300', '02_195_000200', '02_130_000200', '02_130_000300', '02_198_000300', '02_198_940100', '02_198_000100']</t>
         </is>
       </c>
       <c r="L299" t="inlineStr">
@@ -15212,7 +15212,7 @@
       <c r="J300" t="inlineStr"/>
       <c r="K300" t="inlineStr">
         <is>
-          <t>[2811, 2712, 2711, 2812, 2823, 2822, 2714, 2713, 2305, 300, 200, 2502, 2601, 2501, 2821]</t>
+          <t>['02_020_002811', '02_020_002712', '02_020_002711', '02_020_002812', '02_020_002823', '02_020_002822', '02_020_002714', '02_020_002713', '02_020_002305', '02_122_000300', '02_122_000200', '02_020_002502', '02_020_002601', '02_020_002501', '02_020_002821']</t>
         </is>
       </c>
       <c r="L300" t="inlineStr">
@@ -15262,7 +15262,7 @@
       <c r="J301" t="inlineStr"/>
       <c r="K301" t="inlineStr">
         <is>
-          <t>[2811, 2813, 2712, 2812, 2823, 2603, 2822, 980000, 2713, 2601, 2821]</t>
+          <t>['02_020_002811', '02_020_002813', '02_020_002712', '02_020_002812', '02_020_002823', '02_020_002603', '02_020_002822', '02_020_980000', '02_020_002713', '02_020_002601', '02_020_002821']</t>
         </is>
       </c>
       <c r="L301" t="inlineStr">
@@ -15312,7 +15312,7 @@
       <c r="J302" t="inlineStr"/>
       <c r="K302" t="inlineStr">
         <is>
-          <t>[2602, 2811, 2813, 1732, 2812, 2603, 980000, 980200, 1802, 2601, 1602, 1701, 1801]</t>
+          <t>['02_020_002602', '02_020_002811', '02_020_002813', '02_020_001732', '02_020_002812', '02_020_002603', '02_020_980000', '02_020_980200', '02_020_001802', '02_020_002601', '02_020_001602', '02_020_001701', '02_020_001801']</t>
         </is>
       </c>
       <c r="L302" t="inlineStr">
@@ -15362,7 +15362,7 @@
       <c r="J303" t="inlineStr"/>
       <c r="K303" t="inlineStr">
         <is>
-          <t>[2712, 2711, 2305, 2304, 2302, 2502, 1802, 1900, 2601, 2400, 1500, 2501, 1801]</t>
+          <t>['02_020_002712', '02_020_002711', '02_020_002305', '02_020_002304', '02_020_002302', '02_020_002502', '02_020_001802', '02_020_001900', '02_020_002601', '02_020_002400', '02_020_001500', '02_020_002501', '02_020_001801']</t>
         </is>
       </c>
       <c r="L303" t="inlineStr">
@@ -15412,7 +15412,7 @@
       <c r="J304" t="inlineStr"/>
       <c r="K304" t="inlineStr">
         <is>
-          <t>[1300, 902, 1000, 1401, 1402, 2302, 1601, 2502, 1802, 1900, 1602, 2000, 2100, 2400, 1500, 2202, 2501, 1801]</t>
+          <t>['02_020_001300', '02_020_000902', '02_020_001000', '02_020_001401', '02_020_001402', '02_020_002302', '02_020_001601', '02_020_002502', '02_020_001802', '02_020_001900', '02_020_001602', '02_020_002000', '02_020_002100', '02_020_002400', '02_020_001500', '02_020_002202', '02_020_002501', '02_020_001801']</t>
         </is>
       </c>
       <c r="L304" t="inlineStr">
@@ -15462,7 +15462,7 @@
       <c r="J305" t="inlineStr"/>
       <c r="K305" t="inlineStr">
         <is>
-          <t>[2712, 2711, 2301, 2714, 2713, 2305, 2304, 200, 2302]</t>
+          <t>['02_020_002712', '02_020_002711', '02_020_002301', '02_020_002714', '02_020_002713', '02_020_002305', '02_020_002304', '02_122_000200', '02_020_002302']</t>
         </is>
       </c>
       <c r="L305" t="inlineStr">
@@ -15512,7 +15512,7 @@
       <c r="J306" t="inlineStr"/>
       <c r="K306" t="inlineStr">
         <is>
-          <t>[604, 1300, 2711, 1200, 1100, 2301, 2305, 2304, 200, 502, 2302, 2100, 2400, 2201, 2202, 2501, 500]</t>
+          <t>['02_170_000604', '02_020_001300', '02_020_002711', '02_020_001200', '02_020_001100', '02_020_002301', '02_020_002305', '02_020_002304', '02_122_000200', '02_170_000502', '02_020_002302', '02_020_002100', '02_020_002400', '02_020_002201', '02_020_002202', '02_020_002501', '02_020_000500']</t>
         </is>
       </c>
       <c r="L306" t="inlineStr">
@@ -15562,7 +15562,7 @@
       <c r="J307" t="inlineStr"/>
       <c r="K307" t="inlineStr">
         <is>
-          <t>[1300, 902, 901, 1200, 1000, 1100, 1401, 1402, 1601, 2000, 2100, 1500, 2202]</t>
+          <t>['02_020_001300', '02_020_000902', '02_020_000901', '02_020_001200', '02_020_001000', '02_020_001100', '02_020_001401', '02_020_001402', '02_020_001601', '02_020_002000', '02_020_002100', '02_020_001500', '02_020_002202']</t>
         </is>
       </c>
       <c r="L307" t="inlineStr">
@@ -15612,7 +15612,7 @@
       <c r="J308" t="inlineStr"/>
       <c r="K308" t="inlineStr">
         <is>
-          <t>[604, 1300, 703, 801, 702, 901, 701, 204, 1200, 1000, 1100, 980100, 601, 602, 980200, 500]</t>
+          <t>['02_170_000604', '02_020_001300', '02_020_000703', '02_020_000801', '02_020_000702', '02_020_000901', '02_020_000701', '02_020_000204', '02_020_001200', '02_020_001000', '02_020_001100', '02_020_980100', '02_020_000601', '02_020_000602', '02_020_980200', '02_020_000500']</t>
         </is>
       </c>
       <c r="L308" t="inlineStr">
@@ -15662,7 +15662,7 @@
       <c r="J309" t="inlineStr"/>
       <c r="K309" t="inlineStr">
         <is>
-          <t>[801, 802, 902, 901, 980100, 601, 602, 1601, 1602, 1500]</t>
+          <t>['02_020_000801', '02_020_000802', '02_020_000902', '02_020_000901', '02_020_980100', '02_020_000601', '02_020_000602', '02_020_001601', '02_020_001602', '02_020_001500']</t>
         </is>
       </c>
       <c r="L309" t="inlineStr">
@@ -15712,7 +15712,7 @@
       <c r="J310" t="inlineStr"/>
       <c r="K310" t="inlineStr">
         <is>
-          <t>[102, 100, 100, 200, 300, 200, 400, 100, 600, 100, 500, 200, 100, 100, 200]</t>
+          <t>['02_130_000102', '02_100_000100', '02_066_000100', '02_063_000200', '02_275_000300', '02_195_000200', '02_105_000400', '02_282_000100', '02_110_000600', '02_110_000100', '02_110_000500', '02_220_000200', '02_220_000100', '02_198_000100', '02_198_000200']</t>
         </is>
       </c>
       <c r="L310" t="inlineStr">
@@ -15762,7 +15762,7 @@
       <c r="J311" t="inlineStr"/>
       <c r="K311" t="inlineStr">
         <is>
-          <t>[2602, 801, 802, 701, 980000, 1601, 1802, 2601, 1602, 1701, 1702, 1500, 1801]</t>
+          <t>['02_020_002602', '02_020_000801', '02_020_000802', '02_020_000701', '02_020_980000', '02_020_001601', '02_020_001802', '02_020_002601', '02_020_001602', '02_020_001701', '02_020_001702', '02_020_001500', '02_020_001801']</t>
         </is>
       </c>
       <c r="L311" t="inlineStr">
@@ -15812,7 +15812,7 @@
       <c r="J312" t="inlineStr"/>
       <c r="K312" t="inlineStr">
         <is>
-          <t>[703, 801, 802, 1732, 702, 701, 980000, 980200, 1701, 1702, 1731]</t>
+          <t>['02_020_000703', '02_020_000801', '02_020_000802', '02_020_001732', '02_020_000702', '02_020_000701', '02_020_980000', '02_020_980200', '02_020_001701', '02_020_001702', '02_020_001731']</t>
         </is>
       </c>
       <c r="L312" t="inlineStr">
@@ -15862,7 +15862,7 @@
       <c r="J313" t="inlineStr"/>
       <c r="K313" t="inlineStr">
         <is>
-          <t>[703, 801, 802, 702, 701, 602, 980200, 1702, 1731]</t>
+          <t>['02_020_000703', '02_020_000801', '02_020_000802', '02_020_000702', '02_020_000701', '02_020_000602', '02_020_980200', '02_020_001702', '02_020_001731']</t>
         </is>
       </c>
       <c r="L313" t="inlineStr">
@@ -15912,7 +15912,7 @@
       <c r="J314" t="inlineStr"/>
       <c r="K314" t="inlineStr">
         <is>
-          <t>[2813, 703, 1732, 102, 202, 204, 2823, 101, 2900, 205, 980000, 206, 980200, 201, 1731]</t>
+          <t>['02_020_002813', '02_020_000703', '02_020_001732', '02_020_000102', '02_020_000202', '02_020_000204', '02_020_002823', '02_020_000101', '02_020_002900', '02_020_000205', '02_020_980000', '02_020_000206', '02_020_980200', '02_020_000201', '02_020_001731']</t>
         </is>
       </c>
       <c r="L314" t="inlineStr">
@@ -15962,7 +15962,7 @@
       <c r="J315" t="inlineStr"/>
       <c r="K315" t="inlineStr">
         <is>
-          <t>[604, 601, 300, 102, 202, 204, 101, 2900, 980100, 206, 980200, 201, 200, 1300]</t>
+          <t>['02_170_000604', '02_170_000601', '02_063_000300', '02_020_000102', '02_020_000202', '02_020_000204', '02_020_000101', '02_020_002900', '02_020_980100', '02_020_000206', '02_020_980200', '02_020_000201', '02_170_000200', '02_170_001300']</t>
         </is>
       </c>
       <c r="L315" t="inlineStr">
@@ -16012,7 +16012,7 @@
       <c r="J316" t="inlineStr"/>
       <c r="K316" t="inlineStr">
         <is>
-          <t>[1201, 601, 101, 1202, 1100, 200, 1300, 300]</t>
+          <t>['02_170_001201', '02_170_000601', '02_020_000101', '02_170_001202', '02_170_001100', '02_170_000200', '02_170_001300', '02_170_000300']</t>
         </is>
       </c>
       <c r="L316" t="inlineStr">
@@ -16062,7 +16062,7 @@
       <c r="J317" t="inlineStr"/>
       <c r="K317" t="inlineStr">
         <is>
-          <t>[1004, 701, 604, 703, 401, 1201, 601, 102, 101, 980200, 501, 1202, 603, 1100, 1300, 900]</t>
+          <t>['02_170_001004', '02_170_000701', '02_170_000604', '02_170_000703', '02_170_000401', '02_170_001201', '02_170_000601', '02_020_000102', '02_020_000101', '02_020_980200', '02_170_000501', '02_170_001202', '02_170_000603', '02_170_001100', '02_170_001300', '02_170_000900']</t>
         </is>
       </c>
       <c r="L317" t="inlineStr">
@@ -16112,7 +16112,7 @@
       <c r="J318" t="inlineStr"/>
       <c r="K318" t="inlineStr">
         <is>
-          <t>[1004, 701, 604, 705, 703, 402, 401, 706, 601, 501, 1003, 603, 800, 900]</t>
+          <t>['02_170_001004', '02_170_000701', '02_170_000604', '02_170_000705', '02_170_000703', '02_170_000402', '02_170_000401', '02_170_000706', '02_170_000601', '02_170_000501', '02_170_001003', '02_170_000603', '02_170_000800', '02_170_000900']</t>
         </is>
       </c>
       <c r="L318" t="inlineStr">
@@ -16162,7 +16162,7 @@
       <c r="J319" t="inlineStr"/>
       <c r="K319" t="inlineStr">
         <is>
-          <t>[1004, 705, 703, 1001, 706, 601, 1003, 1100, 800, 900]</t>
+          <t>['02_170_001004', '02_170_000705', '02_170_000703', '02_170_001001', '02_170_000706', '02_170_000601', '02_170_001003', '02_170_001100', '02_170_000800', '02_170_000900']</t>
         </is>
       </c>
       <c r="L319" t="inlineStr">
@@ -16212,7 +16212,7 @@
       <c r="J320" t="inlineStr"/>
       <c r="K320" t="inlineStr">
         <is>
-          <t>[1004, 102, 705, 101, 402, 1001, 706, 300, 100, 200, 101, 2900, 1003, 400, 100, 1100, 200, 1300, 300]</t>
+          <t>['02_170_001004', '02_170_000102', '02_170_000705', '02_170_000101', '02_170_000402', '02_170_001001', '02_170_000706', '02_063_000300', '02_066_000100', '02_063_000200', '02_020_000101', '02_020_002900', '02_170_001003', '02_240_000400', '02_068_000100', '02_170_001100', '02_170_000200', '02_170_001300', '02_170_000300']</t>
         </is>
       </c>
       <c r="L320" t="inlineStr">
@@ -16262,7 +16262,7 @@
       <c r="J321" t="inlineStr"/>
       <c r="K321" t="inlineStr">
         <is>
-          <t>[701, 102, 604, 101, 703, 402, 401, 706, 601, 1300, 2301, 980100, 980200, 501, 603, 300, 100, 200, 980000, 502, 400, 400, 200, 100, 300, 500]</t>
+          <t>['02_170_000701', '02_170_000102', '02_170_000604', '02_170_000101', '02_170_000703', '02_170_000402', '02_170_000401', '02_170_000706', '02_170_000601', '02_020_001300', '02_020_002301', '02_020_980100', '02_020_980200', '02_170_000501', '02_170_000603', '02_050_000300', '02_122_000100', '02_122_000200', '02_090_980000', '02_170_000502', '02_240_000400', '02_290_000400', '02_290_000200', '02_068_000100', '02_170_000300', '02_020_000500']</t>
         </is>
       </c>
       <c r="L321" t="inlineStr">
@@ -16312,7 +16312,7 @@
       <c r="J322" t="inlineStr"/>
       <c r="K322" t="inlineStr">
         <is>
-          <t>[100, 300, 400, 700, 1300, 500, 600, 1200, 200, 1000, 800, 980000]</t>
+          <t>['02_090_000100', '02_090_000300', '02_090_000400', '02_090_000700', '02_090_001300', '02_090_000500', '02_090_000600', '02_090_001200', '02_090_000200', '02_090_001000', '02_090_000800', '02_090_980000']</t>
         </is>
       </c>
       <c r="L322" t="inlineStr">
@@ -16362,7 +16362,7 @@
       <c r="J323" t="inlineStr"/>
       <c r="K323" t="inlineStr">
         <is>
-          <t>[100, 300, 400, 1300, 500, 1200, 1600, 1000, 980000, 1402, 1401]</t>
+          <t>['02_090_000100', '02_090_000300', '02_090_000400', '02_090_001300', '02_090_000500', '02_090_001200', '02_090_001600', '02_090_001000', '02_090_980000', '02_090_001402', '02_090_001401']</t>
         </is>
       </c>
       <c r="L323" t="inlineStr">
@@ -16412,7 +16412,7 @@
       <c r="J324" t="inlineStr"/>
       <c r="K324" t="inlineStr">
         <is>
-          <t>[1700, 1200, 1600, 980000, 980100, 1501, 1902, 1402, 1502, 1401]</t>
+          <t>['02_090_001700', '02_090_001200', '02_090_001600', '02_090_980000', '02_090_980100', '02_090_001501', '02_090_001902', '02_090_001402', '02_090_001502', '02_090_001401']</t>
         </is>
       </c>
       <c r="L324" t="inlineStr">
@@ -16462,7 +16462,7 @@
       <c r="J325" t="inlineStr"/>
       <c r="K325" t="inlineStr">
         <is>
-          <t>[100, 1700, 1300, 600, 1200, 1600, 980000, 400, 980100, 1501, 1902, 1502, 1901, 100]</t>
+          <t>['02_240_000100', '02_090_001700', '02_090_001300', '02_090_000600', '02_090_001200', '02_090_001600', '02_090_980000', '02_240_000400', '02_090_980100', '02_090_001501', '02_090_001902', '02_090_001502', '02_090_001901', '02_290_000100']</t>
         </is>
       </c>
       <c r="L325" t="inlineStr">
@@ -16512,7 +16512,7 @@
       <c r="J326" t="inlineStr"/>
       <c r="K326" t="inlineStr">
         <is>
-          <t>[700, 1700, 1300, 600, 200, 1600, 900, 1000, 800, 980000, 400, 980100, 1402, 1901, 200, 100]</t>
+          <t>['02_090_000700', '02_090_001700', '02_090_001300', '02_090_000600', '02_090_000200', '02_090_001600', '02_090_000900', '02_090_001000', '02_090_000800', '02_090_980000', '02_240_000400', '02_090_980100', '02_090_001402', '02_090_001901', '02_290_000200', '02_068_000100']</t>
         </is>
       </c>
       <c r="L326" t="inlineStr">
@@ -16562,7 +16562,7 @@
       <c r="J327" t="inlineStr"/>
       <c r="K327" t="inlineStr">
         <is>
-          <t>[100, 200, 100, 100, 400, 300, 100]</t>
+          <t>['02_180_000100', '02_180_000200', '02_050_000100', '02_158_000100', '02_290_000400', '02_290_000300', '02_188_000100']</t>
         </is>
       </c>
       <c r="L327" t="inlineStr">
@@ -16612,7 +16612,7 @@
       <c r="J328" t="inlineStr"/>
       <c r="K328" t="inlineStr">
         <is>
-          <t>[200, 400, 300, 400, 600, 100, 200, 500]</t>
+          <t>['02_195_000200', '02_105_000400', '02_110_000300', '02_110_000400', '02_110_000600', '02_110_000100', '02_110_000200', '02_110_000500']</t>
         </is>
       </c>
       <c r="L328" t="inlineStr">
@@ -16662,7 +16662,7 @@
       <c r="J329" t="inlineStr"/>
       <c r="K329" t="inlineStr">
         <is>
-          <t>[300, 100, 200, 2900, 300, 400, 1200, 1300, 100, 100, 400, 300, 500, 200]</t>
+          <t>['02_063_000300', '02_066_000100', '02_063_000200', '02_020_002900', '02_122_000300', '02_122_000400', '02_122_001200', '02_122_001300', '02_282_000100', '02_150_000100', '02_150_000400', '02_150_000300', '02_150_000500', '02_150_000200']</t>
         </is>
       </c>
       <c r="L329" t="inlineStr">
@@ -16712,7 +16712,7 @@
       <c r="J330" t="inlineStr"/>
       <c r="K330" t="inlineStr">
         <is>
-          <t>[701, 702, 1000, 800, 100, 900, 1100, 400, 1200, 1300]</t>
+          <t>['02_122_000701', '02_122_000702', '02_122_001000', '02_122_000800', '02_122_000100', '02_122_000900', '02_122_001100', '02_122_000400', '02_122_001200', '02_122_001300']</t>
         </is>
       </c>
       <c r="L330" t="inlineStr">
@@ -16762,7 +16762,7 @@
       <c r="J331" t="inlineStr"/>
       <c r="K331" t="inlineStr">
         <is>
-          <t>[701, 702, 100, 400, 500, 600, 200]</t>
+          <t>['02_122_000701', '02_122_000702', '02_122_000100', '02_122_000400', '02_122_000500', '02_122_000600', '02_122_000200']</t>
         </is>
       </c>
       <c r="L331" t="inlineStr">
@@ -16812,7 +16812,7 @@
       <c r="J332" t="inlineStr"/>
       <c r="K332" t="inlineStr">
         <is>
-          <t>[2813, 300, 204, 2812, 2823, 101, 2822, 2900, 980000, 2713, 980200, 300, 2821]</t>
+          <t>['02_020_002813', '02_063_000300', '02_020_000204', '02_020_002812', '02_020_002823', '02_020_000101', '02_020_002822', '02_020_002900', '02_020_980000', '02_020_002713', '02_020_980200', '02_122_000300', '02_020_002821']</t>
         </is>
       </c>
       <c r="L332" t="inlineStr">
@@ -16862,7 +16862,7 @@
       <c r="J333" t="inlineStr"/>
       <c r="K333" t="inlineStr">
         <is>
-          <t>[1500, 1700, 1800, 1900, 2001, 2002, 2102, 2200]</t>
+          <t>['23_005_001500', '23_005_001700', '23_005_001800', '23_005_001900', '23_005_002001', '23_005_002002', '23_005_002102', '23_005_002200']</t>
         </is>
       </c>
       <c r="L333" t="inlineStr">
@@ -16912,7 +16912,7 @@
       <c r="J334" t="inlineStr"/>
       <c r="K334" t="inlineStr">
         <is>
-          <t>[4402, 4600, 4501, 4502, 4202, 2400, 11500, 4401]</t>
+          <t>['23_005_004402', '23_005_004600', '23_005_004501', '23_005_004502', '23_005_004202', '23_005_002400', '23_005_011500', '23_005_004401']</t>
         </is>
       </c>
       <c r="L334" t="inlineStr">
@@ -16962,7 +16962,7 @@
       <c r="J335" t="inlineStr"/>
       <c r="K335" t="inlineStr">
         <is>
-          <t>[11300, 40000, 4501, 970302, 970301, 4502, 11205, 11204, 11203, 11206]</t>
+          <t>['23_005_011300', '23_001_040000', '23_005_004501', '23_023_970302', '23_023_970301', '23_005_004502', '23_005_011205', '23_005_011204', '23_005_011203', '23_005_011206']</t>
         </is>
       </c>
       <c r="L335" t="inlineStr">
@@ -17012,7 +17012,7 @@
       <c r="J336" t="inlineStr"/>
       <c r="K336" t="inlineStr">
         <is>
-          <t>[971000, 990000, 975500, 975300, 975600, 975700, 975400, 975200, 975100]</t>
+          <t>['23_013_971000', '23_015_990000', '23_015_975500', '23_015_975300', '23_015_975600', '23_015_975700', '23_015_975400', '23_015_975200', '23_015_975100']</t>
         </is>
       </c>
       <c r="L336" t="inlineStr">
@@ -19738,7 +19738,7 @@
       <c r="J392" t="inlineStr"/>
       <c r="K392" t="inlineStr">
         <is>
-          <t>[400, 102, 101, 100, 100, 200, 300, 200, 400, 200, 300, 100, 600, 500, 200, 100, 300, 940100, 100, 200]</t>
+          <t>['02_130_000400', '02_130_000102', '02_130_000101', '02_100_000100', '02_066_000100', '02_063_000200', '02_275_000300', '02_195_000200', '02_105_000400', '02_130_000200', '02_130_000300', '02_282_000100', '02_110_000600', '02_110_000500', '02_220_000200', '02_220_000100', '02_198_000300', '02_198_940100', '02_198_000100', '02_198_000200']</t>
         </is>
       </c>
       <c r="L392" t="inlineStr">
@@ -19790,7 +19790,7 @@
       <c r="J393" t="inlineStr"/>
       <c r="K393" t="inlineStr">
         <is>
-          <t>[701, 702, 300, 100, 200, 2900, 1000, 800, 900, 1100, 300, 400, 1200, 1300, 100, 100, 400, 300, 500, 200]</t>
+          <t>['02_122_000701', '02_122_000702', '02_063_000300', '02_066_000100', '02_063_000200', '02_020_002900', '02_122_001000', '02_122_000800', '02_122_000900', '02_122_001100', '02_122_000300', '02_122_000400', '02_122_001200', '02_122_001300', '02_282_000100', '02_150_000100', '02_150_000400', '02_150_000300', '02_150_000500', '02_150_000200']</t>
         </is>
       </c>
       <c r="L393" t="inlineStr">
@@ -19842,7 +19842,7 @@
       <c r="J394" t="inlineStr"/>
       <c r="K394" t="inlineStr">
         <is>
-          <t>[701, 702, 300, 2900, 300, 400, 500, 600, 200, 1300]</t>
+          <t>['02_122_000701', '02_122_000702', '02_063_000300', '02_020_002900', '02_122_000300', '02_122_000400', '02_122_000500', '02_122_000600', '02_122_000200', '02_122_001300']</t>
         </is>
       </c>
       <c r="L394" t="inlineStr">
@@ -19894,7 +19894,7 @@
       <c r="J395" t="inlineStr"/>
       <c r="K395" t="inlineStr">
         <is>
-          <t>[2811, 2813, 300, 2712, 2711, 204, 2812, 2823, 101, 2822, 2900, 980000, 2714, 2713, 980200, 2305, 300, 2502, 2601, 2501, 2821]</t>
+          <t>['02_020_002811', '02_020_002813', '02_063_000300', '02_020_002712', '02_020_002711', '02_020_000204', '02_020_002812', '02_020_002823', '02_020_000101', '02_020_002822', '02_020_002900', '02_020_980000', '02_020_002714', '02_020_002713', '02_020_980200', '02_020_002305', '02_122_000300', '02_020_002502', '02_020_002601', '02_020_002501', '02_020_002821']</t>
         </is>
       </c>
       <c r="L395" t="inlineStr">
@@ -19946,7 +19946,7 @@
       <c r="J396" t="inlineStr"/>
       <c r="K396" t="inlineStr">
         <is>
-          <t>[2602, 2811, 2813, 1732, 2712, 2812, 2823, 2603, 2822, 980000, 2713, 980200, 1802, 2601, 1602, 1701, 1801, 2821]</t>
+          <t>['02_020_002602', '02_020_002811', '02_020_002813', '02_020_001732', '02_020_002712', '02_020_002812', '02_020_002823', '02_020_002603', '02_020_002822', '02_020_980000', '02_020_002713', '02_020_980200', '02_020_001802', '02_020_002601', '02_020_001602', '02_020_001701', '02_020_001801', '02_020_002821']</t>
         </is>
       </c>
       <c r="L396" t="inlineStr">
@@ -19998,7 +19998,7 @@
       <c r="J397" t="inlineStr"/>
       <c r="K397" t="inlineStr">
         <is>
-          <t>[1300, 902, 2712, 2711, 1000, 1401, 1402, 2305, 2304, 2302, 1601, 2502, 1802, 1900, 2601, 1602, 2000, 2100, 2400, 1500, 2202, 2501, 1801]</t>
+          <t>['02_020_001300', '02_020_000902', '02_020_002712', '02_020_002711', '02_020_001000', '02_020_001401', '02_020_001402', '02_020_002305', '02_020_002304', '02_020_002302', '02_020_001601', '02_020_002502', '02_020_001802', '02_020_001900', '02_020_002601', '02_020_001602', '02_020_002000', '02_020_002100', '02_020_002400', '02_020_001500', '02_020_002202', '02_020_002501', '02_020_001801']</t>
         </is>
       </c>
       <c r="L397" t="inlineStr">
@@ -20050,7 +20050,7 @@
       <c r="J398" t="inlineStr"/>
       <c r="K398" t="inlineStr">
         <is>
-          <t>[1300, 2712, 2711, 1200, 2301, 2714, 2305, 2304, 2302, 2100, 2400, 2201, 2202, 2501]</t>
+          <t>['02_020_001300', '02_020_002712', '02_020_002711', '02_020_001200', '02_020_002301', '02_020_002714', '02_020_002305', '02_020_002304', '02_020_002302', '02_020_002100', '02_020_002400', '02_020_002201', '02_020_002202', '02_020_002501']</t>
         </is>
       </c>
       <c r="L398" t="inlineStr">
@@ -20102,7 +20102,7 @@
       <c r="J399" t="inlineStr"/>
       <c r="K399" t="inlineStr">
         <is>
-          <t>[1300, 703, 801, 902, 702, 901, 701, 204, 1200, 1000, 1100, 980100, 1401, 601, 602, 980200, 1402, 1601, 2000, 2100, 1500, 2202, 500]</t>
+          <t>['02_020_001300', '02_020_000703', '02_020_000801', '02_020_000902', '02_020_000702', '02_020_000901', '02_020_000701', '02_020_000204', '02_020_001200', '02_020_001000', '02_020_001100', '02_020_980100', '02_020_001401', '02_020_000601', '02_020_000602', '02_020_980200', '02_020_001402', '02_020_001601', '02_020_002000', '02_020_002100', '02_020_001500', '02_020_002202', '02_020_000500']</t>
         </is>
       </c>
       <c r="L399" t="inlineStr">
@@ -20154,7 +20154,7 @@
       <c r="J400" t="inlineStr"/>
       <c r="K400" t="inlineStr">
         <is>
-          <t>[2602, 801, 802, 902, 901, 701, 980100, 980000, 601, 602, 1601, 1802, 2601, 1602, 1701, 1702, 1500, 1801]</t>
+          <t>['02_020_002602', '02_020_000801', '02_020_000802', '02_020_000902', '02_020_000901', '02_020_000701', '02_020_980100', '02_020_980000', '02_020_000601', '02_020_000602', '02_020_001601', '02_020_001802', '02_020_002601', '02_020_001602', '02_020_001701', '02_020_001702', '02_020_001500', '02_020_001801']</t>
         </is>
       </c>
       <c r="L400" t="inlineStr">
@@ -20206,7 +20206,7 @@
       <c r="J401" t="inlineStr"/>
       <c r="K401" t="inlineStr">
         <is>
-          <t>[703, 801, 802, 1732, 702, 701, 980000, 602, 980200, 1701, 1702, 1731]</t>
+          <t>['02_020_000703', '02_020_000801', '02_020_000802', '02_020_001732', '02_020_000702', '02_020_000701', '02_020_980000', '02_020_000602', '02_020_980200', '02_020_001701', '02_020_001702', '02_020_001731']</t>
         </is>
       </c>
       <c r="L401" t="inlineStr">
@@ -20258,7 +20258,7 @@
       <c r="J402" t="inlineStr"/>
       <c r="K402" t="inlineStr">
         <is>
-          <t>[2813, 601, 300, 703, 1732, 102, 202, 204, 2823, 101, 2900, 980100, 205, 980000, 206, 980200, 201, 200, 1300, 1731]</t>
+          <t>['02_020_002813', '02_170_000601', '02_063_000300', '02_020_000703', '02_020_001732', '02_020_000102', '02_020_000202', '02_020_000204', '02_020_002823', '02_020_000101', '02_020_002900', '02_020_980100', '02_020_000205', '02_020_980000', '02_020_000206', '02_020_980200', '02_020_000201', '02_170_000200', '02_170_001300', '02_020_001731']</t>
         </is>
       </c>
       <c r="L402" t="inlineStr">
@@ -20310,7 +20310,7 @@
       <c r="J403" t="inlineStr"/>
       <c r="K403" t="inlineStr">
         <is>
-          <t>[1004, 701, 604, 703, 401, 1201, 601, 101, 501, 1202, 603, 1100, 200, 1300, 300, 900]</t>
+          <t>['02_170_001004', '02_170_000701', '02_170_000604', '02_170_000703', '02_170_000401', '02_170_001201', '02_170_000601', '02_020_000101', '02_170_000501', '02_170_001202', '02_170_000603', '02_170_001100', '02_170_000200', '02_170_001300', '02_170_000300', '02_170_000900']</t>
         </is>
       </c>
       <c r="L403" t="inlineStr">
@@ -20362,7 +20362,7 @@
       <c r="J404" t="inlineStr"/>
       <c r="K404" t="inlineStr">
         <is>
-          <t>[1004, 701, 604, 705, 703, 402, 1001, 401, 706, 601, 501, 1003, 603, 1100, 800, 900]</t>
+          <t>['02_170_001004', '02_170_000701', '02_170_000604', '02_170_000705', '02_170_000703', '02_170_000402', '02_170_001001', '02_170_000401', '02_170_000706', '02_170_000601', '02_170_000501', '02_170_001003', '02_170_000603', '02_170_001100', '02_170_000800', '02_170_000900']</t>
         </is>
       </c>
       <c r="L404" t="inlineStr">
@@ -20414,7 +20414,7 @@
       <c r="J405" t="inlineStr"/>
       <c r="K405" t="inlineStr">
         <is>
-          <t>[1004, 701, 102, 604, 705, 101, 703, 402, 1001, 401, 706, 300, 100, 200, 101, 2900, 501, 1003, 603, 300, 100, 980000, 502, 400, 400, 200, 100, 1100, 200, 1300, 300]</t>
+          <t>['02_170_001004', '02_170_000701', '02_170_000102', '02_170_000604', '02_170_000705', '02_170_000101', '02_170_000703', '02_170_000402', '02_170_001001', '02_170_000401', '02_170_000706', '02_063_000300', '02_066_000100', '02_063_000200', '02_020_000101', '02_020_002900', '02_170_000501', '02_170_001003', '02_170_000603', '02_050_000300', '02_122_000100', '02_090_980000', '02_170_000502', '02_240_000400', '02_290_000400', '02_290_000200', '02_068_000100', '02_170_001100', '02_170_000200', '02_170_001300', '02_170_000300']</t>
         </is>
       </c>
       <c r="L405" t="inlineStr">
@@ -20466,7 +20466,7 @@
       <c r="J406" t="inlineStr"/>
       <c r="K406" t="inlineStr">
         <is>
-          <t>[100, 300, 400, 700, 1300, 500, 600, 1200, 200, 1600, 1000, 800, 980000, 1402, 1401]</t>
+          <t>['02_090_000100', '02_090_000300', '02_090_000400', '02_090_000700', '02_090_001300', '02_090_000500', '02_090_000600', '02_090_001200', '02_090_000200', '02_090_001600', '02_090_001000', '02_090_000800', '02_090_980000', '02_090_001402', '02_090_001401']</t>
         </is>
       </c>
       <c r="L406" t="inlineStr">
@@ -20518,7 +20518,7 @@
       <c r="J407" t="inlineStr"/>
       <c r="K407" t="inlineStr">
         <is>
-          <t>[100, 1700, 1300, 600, 1200, 1600, 980000, 400, 980100, 1501, 1902, 1402, 1502, 1901, 1401, 100]</t>
+          <t>['02_240_000100', '02_090_001700', '02_090_001300', '02_090_000600', '02_090_001200', '02_090_001600', '02_090_980000', '02_240_000400', '02_090_980100', '02_090_001501', '02_090_001902', '02_090_001402', '02_090_001502', '02_090_001901', '02_090_001401', '02_290_000100']</t>
         </is>
       </c>
       <c r="L407" t="inlineStr">
@@ -20570,7 +20570,7 @@
       <c r="J408" t="inlineStr"/>
       <c r="K408" t="inlineStr">
         <is>
-          <t>[100, 101, 100, 300, 100, 200, 200, 300, 700, 1700, 1300, 600, 200, 1600, 900, 1000, 800, 980000, 400, 100, 100, 980100, 1902, 1402, 1901, 400, 100, 200, 300, 100, 200, 100]</t>
+          <t>['02_240_000100', '02_170_000101', '02_180_000100', '02_063_000300', '02_066_000100', '02_063_000200', '02_185_000200', '02_050_000300', '02_090_000700', '02_090_001700', '02_090_001300', '02_090_000600', '02_090_000200', '02_090_001600', '02_090_000900', '02_090_001000', '02_090_000800', '02_090_980000', '02_240_000400', '02_158_000100', '02_282_000100', '02_090_980100', '02_090_001902', '02_090_001402', '02_090_001901', '02_290_000400', '02_290_000100', '02_290_000200', '02_290_000300', '02_068_000100', '02_170_000200', '02_188_000100']</t>
         </is>
       </c>
       <c r="L408" t="inlineStr">
@@ -20622,7 +20622,7 @@
       <c r="J409" t="inlineStr"/>
       <c r="K409" t="inlineStr">
         <is>
-          <t>[101, 100, 200, 300, 100, 100, 1200, 100, 200, 100, 100, 200, 100, 400, 100, 100]</t>
+          <t>['02_170_000101', '02_013_000100', '02_050_000200', '02_050_000300', '02_050_000100', '02_122_000100', '02_122_001200', '02_164_000100', '02_016_000200', '02_016_000100', '02_158_000100', '02_070_000200', '02_070_000100', '02_290_000400', '02_150_000100', '02_060_000100']</t>
         </is>
       </c>
       <c r="L409" t="inlineStr">
@@ -20672,7 +20672,7 @@
       <c r="J410" t="inlineStr"/>
       <c r="K410" t="inlineStr">
         <is>
-          <t>[3000, 12000, 43000, 2000, 970200, 19000, 20500, 965300, 965400, 970302, 970301, 12500, 971100, 45000, 41000, 42000, 44000, 47000, 966000, 21000, 20000, 965800, 46002, 46001, 975100]</t>
+          <t>['23_019_003000', '23_019_012000', '23_027_043000', '23_019_002000', '23_013_970200', '23_011_019000', '23_011_020500', '23_009_965300', '23_009_965400', '23_013_970302', '23_013_970301', '23_019_012500', '23_013_971100', '23_027_045000', '23_027_041000', '23_027_042000', '23_027_044000', '23_027_047000', '23_025_966000', '23_011_021000', '23_011_020000', '23_025_965800', '23_027_046002', '23_027_046001', '23_015_975100']</t>
         </is>
       </c>
       <c r="L410" t="inlineStr">

</xml_diff>